<commit_message>
Skip the header row
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCS\JAVA\File-reader\fileReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE42E0B4-EED0-4D3B-AC90-A33B1A417B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53517172-B293-4428-8AFE-6D44EC7C3833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B024CA4C-988F-4558-B3D3-A4B8A87B7F7D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>Name one</t>
   </si>
@@ -117,13 +117,28 @@
   </si>
   <si>
     <t>depart4</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Department</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +150,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,6 +201,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -493,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19AE1C5-878A-43C4-A4F3-DD4D970180B1}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,68 +535,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="6">
-        <v>55</v>
-      </c>
-      <c r="D1" s="4">
-        <v>15000</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D2" s="4">
-        <v>60000</v>
+        <v>15000</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="6">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D3" s="4">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D4" s="4">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>23</v>
@@ -578,16 +604,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>23</v>
@@ -595,13 +621,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D6" s="4">
         <v>60000</v>
@@ -612,84 +638,84 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="6">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D7" s="4">
         <v>60000</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="D8" s="4">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D9" s="4">
-        <v>23456</v>
+        <v>15000</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="6">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4">
-        <v>12443</v>
+        <v>23456</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D11" s="4">
-        <v>74743</v>
+        <v>12443</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
@@ -697,89 +723,106 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C12" s="6">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D12" s="4">
-        <v>60000</v>
+        <v>74743</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="6">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4">
         <v>60000</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="6">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D14" s="4">
-        <v>74782</v>
+        <v>60000</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="6">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D15" s="4">
-        <v>60000</v>
+        <v>74782</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6">
+        <v>45</v>
+      </c>
+      <c r="D16" s="4">
+        <v>60000</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" xr:uid="{64CDCDFA-E083-4AD4-97B3-45B49EF48AF7}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{4E9ED4ED-293B-4243-B729-50B0CC0ED3D2}"/>
-    <hyperlink ref="B13" r:id="rId3" xr:uid="{1E0E8F92-62DD-480E-B6DD-4455BEE51036}"/>
-    <hyperlink ref="B12" r:id="rId4" xr:uid="{534DEBB6-7E8A-4075-B9E7-0E23DAD219B0}"/>
-    <hyperlink ref="B10" r:id="rId5" xr:uid="{2AFDE67F-7AE1-4276-A4A5-D5FFA3046065}"/>
-    <hyperlink ref="B9" r:id="rId6" xr:uid="{3F293EE7-7CEC-4B43-84C5-890B3C5E9ACD}"/>
-    <hyperlink ref="B1" r:id="rId7" xr:uid="{1EBF303A-81E4-4942-BE9E-37E09E9A3534}"/>
-    <hyperlink ref="B3" r:id="rId8" xr:uid="{85638E6F-0CEA-4278-9BEC-389D11300FC7}"/>
-    <hyperlink ref="B5" r:id="rId9" xr:uid="{AB0D29A9-06A0-4AB2-96EC-A44EDDB2B925}"/>
-    <hyperlink ref="B8" r:id="rId10" xr:uid="{327DFE22-25CB-4EBC-A7BB-31C0CB5D1352}"/>
-    <hyperlink ref="B2" r:id="rId11" xr:uid="{12BF8E04-1933-4ABA-B0B3-CB906E675AE9}"/>
-    <hyperlink ref="B4" r:id="rId12" xr:uid="{BD591081-9A3A-4918-97F4-A8A9CFD6A5EB}"/>
-    <hyperlink ref="B11" r:id="rId13" xr:uid="{4828E7D6-E4DF-4165-A594-1509AB0DDA47}"/>
-    <hyperlink ref="B6" r:id="rId14" xr:uid="{89CB5684-AB7D-487C-9DEB-4AAA25B66E4C}"/>
-    <hyperlink ref="B7" r:id="rId15" xr:uid="{0B8ADEAF-2790-4137-BBA5-9160F103139B}"/>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{64CDCDFA-E083-4AD4-97B3-45B49EF48AF7}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{4E9ED4ED-293B-4243-B729-50B0CC0ED3D2}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{1E0E8F92-62DD-480E-B6DD-4455BEE51036}"/>
+    <hyperlink ref="B13" r:id="rId4" xr:uid="{534DEBB6-7E8A-4075-B9E7-0E23DAD219B0}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{2AFDE67F-7AE1-4276-A4A5-D5FFA3046065}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{3F293EE7-7CEC-4B43-84C5-890B3C5E9ACD}"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{1EBF303A-81E4-4942-BE9E-37E09E9A3534}"/>
+    <hyperlink ref="B4" r:id="rId8" xr:uid="{85638E6F-0CEA-4278-9BEC-389D11300FC7}"/>
+    <hyperlink ref="B6" r:id="rId9" xr:uid="{AB0D29A9-06A0-4AB2-96EC-A44EDDB2B925}"/>
+    <hyperlink ref="B9" r:id="rId10" xr:uid="{327DFE22-25CB-4EBC-A7BB-31C0CB5D1352}"/>
+    <hyperlink ref="B3" r:id="rId11" xr:uid="{12BF8E04-1933-4ABA-B0B3-CB906E675AE9}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{BD591081-9A3A-4918-97F4-A8A9CFD6A5EB}"/>
+    <hyperlink ref="B12" r:id="rId13" xr:uid="{4828E7D6-E4DF-4165-A594-1509AB0DDA47}"/>
+    <hyperlink ref="B7" r:id="rId14" xr:uid="{89CB5684-AB7D-487C-9DEB-4AAA25B66E4C}"/>
+    <hyperlink ref="B8" r:id="rId15" xr:uid="{0B8ADEAF-2790-4137-BBA5-9160F103139B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>

</xml_diff>

<commit_message>
Reading the file, validating data, writing the data
Now, the application is reading the xlsx file, validating the data and writing in two separate txt files.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCS\JAVA\File-reader\fileReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53517172-B293-4428-8AFE-6D44EC7C3833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20C9A3C-0B9C-495E-BDAA-5FE021421AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B024CA4C-988F-4558-B3D3-A4B8A87B7F7D}"/>
   </bookViews>
@@ -33,40 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
-  <si>
-    <t>Name one</t>
-  </si>
-  <si>
-    <t>Name Three</t>
-  </si>
-  <si>
-    <t>N5</t>
-  </si>
-  <si>
-    <t>Name Seven</t>
-  </si>
-  <si>
-    <t>Eight</t>
-  </si>
-  <si>
-    <t>nine</t>
-  </si>
-  <si>
-    <t>Ten</t>
-  </si>
-  <si>
-    <t>Twelve</t>
-  </si>
-  <si>
-    <t>Thirteen</t>
-  </si>
-  <si>
-    <t>Fourteen</t>
-  </si>
-  <si>
-    <t>Fifteen</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Fifteen@fiv.com</t>
   </si>
@@ -83,18 +50,9 @@
     <t>Ten@c.com</t>
   </si>
   <si>
-    <t>Nine@c.com</t>
-  </si>
-  <si>
-    <t>N1@a.com</t>
-  </si>
-  <si>
     <t>N3@</t>
   </si>
   <si>
-    <t>N5@.com</t>
-  </si>
-  <si>
     <t>Eight@.com</t>
   </si>
   <si>
@@ -110,12 +68,6 @@
     <t>Dept 4</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>name@.com</t>
-  </si>
-  <si>
     <t>depart4</t>
   </si>
   <si>
@@ -132,6 +84,78 @@
   </si>
   <si>
     <t>Department</t>
+  </si>
+  <si>
+    <t>twenty</t>
+  </si>
+  <si>
+    <t>50000.00</t>
+  </si>
+  <si>
+    <t>Employee one</t>
+  </si>
+  <si>
+    <t>Employee three</t>
+  </si>
+  <si>
+    <t>Employee four</t>
+  </si>
+  <si>
+    <t>Employee five</t>
+  </si>
+  <si>
+    <t>Employee six</t>
+  </si>
+  <si>
+    <t>Employee seven</t>
+  </si>
+  <si>
+    <t>Employee nine</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Employee ten</t>
+  </si>
+  <si>
+    <t>Employee eleven</t>
+  </si>
+  <si>
+    <t>Employee twelve</t>
+  </si>
+  <si>
+    <t>Employee 13</t>
+  </si>
+  <si>
+    <t>Employee fourteen</t>
+  </si>
+  <si>
+    <t>Employee fiften</t>
+  </si>
+  <si>
+    <t>emp_one@a.com</t>
+  </si>
+  <si>
+    <t>empTwo@e.com</t>
+  </si>
+  <si>
+    <t>80.00</t>
+  </si>
+  <si>
+    <t>four@.com</t>
+  </si>
+  <si>
+    <t>Five@.com</t>
+  </si>
+  <si>
+    <t>XX@.com</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>5248</t>
   </si>
 </sst>
 </file>
@@ -184,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,17 +217,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -522,288 +538,278 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>32</v>
+      <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6">
+      <c r="D2" s="1">
+        <v>15000</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1">
         <v>55</v>
       </c>
-      <c r="D2" s="4">
-        <v>15000</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="6">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4">
-        <v>60000</v>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="6">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
         <v>35</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>40000</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1">
         <v>20</v>
       </c>
-      <c r="C5" s="6">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4">
-        <v>50000</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1">
         <v>55</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>60000</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="6">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1">
         <v>76</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>60000</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="6">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1">
         <v>33</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>60000</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
         <v>60</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>15000</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1">
         <v>45</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>23456</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
         <v>65</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="1">
         <v>12443</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="6">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
         <v>44</v>
       </c>
-      <c r="D12" s="4">
-        <v>74743</v>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
         <v>32</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="1">
         <v>60000</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
         <v>33</v>
       </c>
-      <c r="D14" s="4">
-        <v>60000</v>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
         <v>22</v>
       </c>
-      <c r="D15" s="4">
-        <v>74782</v>
+      <c r="D15" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
         <v>45</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="1">
         <v>60000</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -813,18 +819,16 @@
     <hyperlink ref="B14" r:id="rId3" xr:uid="{1E0E8F92-62DD-480E-B6DD-4455BEE51036}"/>
     <hyperlink ref="B13" r:id="rId4" xr:uid="{534DEBB6-7E8A-4075-B9E7-0E23DAD219B0}"/>
     <hyperlink ref="B11" r:id="rId5" xr:uid="{2AFDE67F-7AE1-4276-A4A5-D5FFA3046065}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{3F293EE7-7CEC-4B43-84C5-890B3C5E9ACD}"/>
-    <hyperlink ref="B2" r:id="rId7" xr:uid="{1EBF303A-81E4-4942-BE9E-37E09E9A3534}"/>
-    <hyperlink ref="B4" r:id="rId8" xr:uid="{85638E6F-0CEA-4278-9BEC-389D11300FC7}"/>
-    <hyperlink ref="B6" r:id="rId9" xr:uid="{AB0D29A9-06A0-4AB2-96EC-A44EDDB2B925}"/>
-    <hyperlink ref="B9" r:id="rId10" xr:uid="{327DFE22-25CB-4EBC-A7BB-31C0CB5D1352}"/>
-    <hyperlink ref="B3" r:id="rId11" xr:uid="{12BF8E04-1933-4ABA-B0B3-CB906E675AE9}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{BD591081-9A3A-4918-97F4-A8A9CFD6A5EB}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{1EBF303A-81E4-4942-BE9E-37E09E9A3534}"/>
+    <hyperlink ref="B4" r:id="rId7" xr:uid="{85638E6F-0CEA-4278-9BEC-389D11300FC7}"/>
+    <hyperlink ref="B6" r:id="rId8" xr:uid="{AB0D29A9-06A0-4AB2-96EC-A44EDDB2B925}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{327DFE22-25CB-4EBC-A7BB-31C0CB5D1352}"/>
+    <hyperlink ref="B3" r:id="rId10" xr:uid="{12BF8E04-1933-4ABA-B0B3-CB906E675AE9}"/>
+    <hyperlink ref="B5" r:id="rId11" xr:uid="{BD591081-9A3A-4918-97F4-A8A9CFD6A5EB}"/>
+    <hyperlink ref="B7" r:id="rId12" xr:uid="{89CB5684-AB7D-487C-9DEB-4AAA25B66E4C}"/>
     <hyperlink ref="B12" r:id="rId13" xr:uid="{4828E7D6-E4DF-4165-A594-1509AB0DDA47}"/>
-    <hyperlink ref="B7" r:id="rId14" xr:uid="{89CB5684-AB7D-487C-9DEB-4AAA25B66E4C}"/>
-    <hyperlink ref="B8" r:id="rId15" xr:uid="{0B8ADEAF-2790-4137-BBA5-9160F103139B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>